<commit_message>
Extracted Functions used on the Bottom Board
</commit_message>
<xml_diff>
--- a/pin_outs_X7.xlsx
+++ b/pin_outs_X7.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\IEEE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\X7-hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
   <si>
     <t xml:space="preserve">Pin outs </t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>RS485 B</t>
+  </si>
+  <si>
+    <t>Clockwise from notch</t>
+  </si>
+  <si>
+    <t>?"{{"{{{-*</t>
   </si>
 </sst>
 </file>
@@ -515,12 +521,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,6 +539,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,6 +549,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -830,37 +836,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35:U35"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="20" max="20" width="10" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -877,63 +887,63 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="9" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="H5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="11"/>
-      <c r="O5" s="9" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="O5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="11"/>
-      <c r="W5" s="7" t="s">
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="9"/>
+      <c r="W5" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
       <c r="AA5" s="1"/>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="14"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="12"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
       <c r="AA6" s="1"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -959,12 +969,12 @@
         <v>2</v>
       </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
       <c r="N8" s="2"/>
       <c r="O8" s="6" t="s">
         <v>2</v>
@@ -1538,15 +1548,15 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="O24" s="9" t="s">
+      <c r="O24" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="11"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="9"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1565,13 +1575,13 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="14"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="12"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -1649,7 +1659,7 @@
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
       <c r="T28" s="6" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="U28" s="6"/>
     </row>
@@ -1961,6 +1971,9 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
+      <c r="R40" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
@@ -2228,52 +2241,164 @@
     </row>
   </sheetData>
   <mergeCells count="228">
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="T35:U35"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:S32"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="O24:U25"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="W5:Z6"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="H5:M6"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="O5:U6"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="C9:F9"/>
@@ -2298,164 +2423,52 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="H5:M6"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="O5:U6"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="W5:Z6"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="O24:U25"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="T35:U35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
STM board can now control servo
</commit_message>
<xml_diff>
--- a/pin_outs_X7.xlsx
+++ b/pin_outs_X7.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
   <si>
     <t xml:space="preserve">Pin outs </t>
   </si>
@@ -336,9 +336,6 @@
   </si>
   <si>
     <t>Clockwise from notch</t>
-  </si>
-  <si>
-    <t>?"{{"{{{-*</t>
   </si>
 </sst>
 </file>
@@ -518,7 +515,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -539,9 +542,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,9 +549,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -836,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
@@ -847,30 +844,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -887,63 +884,63 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="H5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="H5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
-      <c r="O5" s="7" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+      <c r="O5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="9"/>
-      <c r="W5" s="13" t="s">
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="11"/>
+      <c r="W5" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
       <c r="AA5" s="1"/>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="12"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="12"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="14"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
       <c r="AA6" s="1"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -955,400 +952,400 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="H8" s="6" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="14" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6" t="s">
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6" t="s">
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="U8" s="6"/>
-      <c r="W8" s="6" t="s">
+      <c r="U8" s="7"/>
+      <c r="W8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6" t="s">
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Z8" s="6"/>
+      <c r="Z8" s="7"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="6">
+      <c r="O9" s="7">
         <v>1</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6" t="s">
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6" t="s">
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U9" s="6"/>
-      <c r="W9" s="6">
+      <c r="U9" s="7"/>
+      <c r="W9" s="7">
         <v>1</v>
       </c>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6" t="s">
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="Z9" s="6"/>
+      <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="H10" s="6" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="O10" s="6">
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="O10" s="7">
         <v>2</v>
       </c>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6" t="s">
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6" t="s">
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U10" s="6"/>
-      <c r="W10" s="6">
+      <c r="U10" s="7"/>
+      <c r="W10" s="7">
         <v>2</v>
       </c>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6" t="s">
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="Z10" s="6"/>
+      <c r="Z10" s="7"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="H11" s="6" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="H11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="O11" s="6">
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="O11" s="7">
         <v>3</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6" t="s">
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6" t="s">
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U11" s="6"/>
-      <c r="W11" s="6">
+      <c r="U11" s="7"/>
+      <c r="W11" s="7">
         <v>3</v>
       </c>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6" t="s">
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="Z11" s="6"/>
+      <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="H12" s="6" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="H12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="O12" s="6">
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="O12" s="7">
         <v>4</v>
       </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6" t="s">
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6" t="s">
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U12" s="6"/>
-      <c r="W12" s="6">
+      <c r="U12" s="7"/>
+      <c r="W12" s="7">
         <v>4</v>
       </c>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6" t="s">
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="Z12" s="6"/>
+      <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="O13" s="6">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="O13" s="7">
         <v>5</v>
       </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6" t="s">
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6">
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7">
         <v>8</v>
       </c>
-      <c r="U13" s="6"/>
-      <c r="W13" s="6">
+      <c r="U13" s="7"/>
+      <c r="W13" s="7">
         <v>5</v>
       </c>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6" t="s">
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="Z13" s="6"/>
+      <c r="Z13" s="7"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="H14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="O14" s="6">
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="O14" s="7">
         <v>6</v>
       </c>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6" t="s">
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6">
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7">
         <v>7</v>
       </c>
-      <c r="U14" s="6"/>
-      <c r="W14" s="6">
+      <c r="U14" s="7"/>
+      <c r="W14" s="7">
         <v>6</v>
       </c>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6" t="s">
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="Z14" s="6"/>
+      <c r="Z14" s="7"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="H15" s="6" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6" t="s">
+      <c r="I15" s="7"/>
+      <c r="J15" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="O15" s="6">
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="O15" s="7">
         <v>7</v>
       </c>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6" t="s">
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6">
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7">
         <v>6</v>
       </c>
-      <c r="U15" s="6"/>
-      <c r="W15" s="6">
+      <c r="U15" s="7"/>
+      <c r="W15" s="7">
         <v>7</v>
       </c>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6" t="s">
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Z15" s="6"/>
+      <c r="Z15" s="7"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="H16" s="6" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6" t="s">
+      <c r="I16" s="7"/>
+      <c r="J16" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="O16" s="6">
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="O16" s="7">
         <v>8</v>
       </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6" t="s">
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6">
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7">
         <v>5</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="W16" s="6">
+      <c r="U16" s="7"/>
+      <c r="W16" s="7">
         <v>8</v>
       </c>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6" t="s">
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="Z16" s="6"/>
+      <c r="Z16" s="7"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="6" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="H17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6" t="s">
+      <c r="I17" s="7"/>
+      <c r="J17" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="O17" s="6">
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="O17" s="7">
         <v>9</v>
       </c>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6" t="s">
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6">
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7">
         <v>4</v>
       </c>
-      <c r="U17" s="6"/>
+      <c r="U17" s="7"/>
       <c r="V17" s="5"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -1357,623 +1354,620 @@
       <c r="AA17" s="1"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6" t="s">
+      <c r="I18" s="7"/>
+      <c r="J18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="O18" s="6">
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="O18" s="7">
         <v>10</v>
       </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6" t="s">
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6">
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7">
         <v>3</v>
       </c>
-      <c r="U18" s="6"/>
+      <c r="U18" s="7"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="O19" s="6">
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="O19" s="7">
         <v>11</v>
       </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6" t="s">
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6">
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7">
         <v>2</v>
       </c>
-      <c r="U19" s="6"/>
+      <c r="U19" s="7"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="H20" s="6" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="O20" s="6">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="O20" s="7">
         <v>12</v>
       </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6" t="s">
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6">
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7">
         <v>1</v>
       </c>
-      <c r="U20" s="6"/>
+      <c r="U20" s="7"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="H21" s="6" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="H21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="O21" s="6">
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="O21" s="7">
         <v>13</v>
       </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6" t="s">
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6">
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7">
         <v>0</v>
       </c>
-      <c r="U21" s="6"/>
+      <c r="U21" s="7"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="H22" s="6" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="H22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="O22" s="6">
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="O22" s="7">
         <v>14</v>
       </c>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6" t="s">
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6" t="s">
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U22" s="6"/>
+      <c r="U22" s="7"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="H23" s="6" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="H23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="H24" s="6" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="H24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="O24" s="7" t="s">
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="O24" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="9"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="11"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="6" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="H25" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="12"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="14"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="H26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="H26" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="H27" s="6" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="H27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="O27" s="6" t="s">
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="O27" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6" t="s">
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6" t="s">
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="U27" s="6"/>
+      <c r="U27" s="7"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="H28" s="6" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="H28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="O28" s="6">
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="O28" s="7">
         <v>1</v>
       </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6" t="s">
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6" t="s">
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="U28" s="6"/>
+      <c r="U28" s="7"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="H29" s="6" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="H29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="O29" s="6">
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="O29" s="7">
         <v>2</v>
       </c>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6" t="s">
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6" t="s">
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U29" s="6"/>
+      <c r="U29" s="7"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="H30" s="6" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="H30" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="O30" s="6">
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="O30" s="7">
         <v>3</v>
       </c>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6" t="s">
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6" t="s">
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U30" s="6"/>
+      <c r="U30" s="7"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="H31" s="6" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="H31" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6" t="s">
+      <c r="I31" s="7"/>
+      <c r="J31" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="O31" s="6">
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="O31" s="7">
         <v>4</v>
       </c>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6" t="s">
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6" t="s">
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U31" s="6"/>
+      <c r="U31" s="7"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="H32" s="6" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="H32" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="O32" s="6">
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="O32" s="7">
         <v>5</v>
       </c>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6" t="s">
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6" t="s">
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U32" s="6"/>
+      <c r="U32" s="7"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="H33" s="6" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="H33" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="O33" s="6">
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="O33" s="7">
         <v>6</v>
       </c>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6" t="s">
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6" t="s">
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U33" s="6"/>
+      <c r="U33" s="7"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="H34" s="6" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="H34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="O34" s="6">
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="O34" s="7">
         <v>7</v>
       </c>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6" t="s">
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6" t="s">
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U34" s="6"/>
+      <c r="U34" s="7"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="H35" s="6" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="H35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="O35" s="6">
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="O35" s="7">
         <v>8</v>
       </c>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6" t="s">
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6"/>
-      <c r="T35" s="6" t="s">
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="U35" s="6"/>
+      <c r="U35" s="7"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="H36" s="6" t="s">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="H36" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="H37" s="6" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="H37" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="H38" s="6" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="H38" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="H39" s="6" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="H39" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="H40" s="6" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="H40" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="R40" t="s">
-        <v>104</v>
-      </c>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
@@ -2241,27 +2235,189 @@
     </row>
   </sheetData>
   <mergeCells count="228">
-    <mergeCell ref="W5:Z6"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="O24:U25"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="H5:M6"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="O5:U6"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="T20:U20"/>
     <mergeCell ref="T21:U21"/>
     <mergeCell ref="T22:U22"/>
@@ -2286,189 +2442,27 @@
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="H5:M6"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="O5:U6"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A5:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="O24:U25"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:S32"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="T34:U34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="T35:U35"/>
+    <mergeCell ref="W5:Z6"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="W16:X16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>